<commit_message>
Soporte para calculo automatico de mejor winrate
</commit_message>
<xml_diff>
--- a/src/ar/edu/unrc/game2048/performanceandtraining/resources/Estadisticas.xlsx
+++ b/src/ar/edu/unrc/game2048/performanceandtraining/resources/Estadisticas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Max Tile" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">Win%</t>
   </si>
   <si>
+    <t xml:space="preserve">Max</t>
+  </si>
+  <si>
     <t xml:space="preserve">Turn</t>
   </si>
 </sst>
@@ -53,12 +56,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -96,6 +100,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -121,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -134,6 +144,13 @@
       <right style="hair"/>
       <top style="hair"/>
       <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -162,7 +179,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -183,15 +200,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -12047,11 +12080,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="91657086"/>
-        <c:axId val="83595348"/>
+        <c:axId val="98603180"/>
+        <c:axId val="91568754"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="91657086"/>
+        <c:axId val="98603180"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12086,14 +12119,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83595348"/>
+        <c:crossAx val="91568754"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83595348"/>
+        <c:axId val="91568754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12108,7 +12141,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12137,7 +12170,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91657086"/>
+        <c:crossAx val="98603180"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14194,11 +14227,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="15285809"/>
-        <c:axId val="91058363"/>
+        <c:axId val="78133733"/>
+        <c:axId val="26654462"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15285809"/>
+        <c:axId val="78133733"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14233,14 +14266,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91058363"/>
+        <c:crossAx val="26654462"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91058363"/>
+        <c:axId val="26654462"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14255,7 +14288,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -14284,7 +14317,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15285809"/>
+        <c:crossAx val="78133733"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -31507,11 +31540,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="71572920"/>
-        <c:axId val="11502199"/>
+        <c:axId val="98575853"/>
+        <c:axId val="61709329"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71572920"/>
+        <c:axId val="98575853"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -31546,14 +31579,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11502199"/>
+        <c:crossAx val="61709329"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11502199"/>
+        <c:axId val="61709329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -31568,7 +31601,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -31597,7 +31630,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71572920"/>
+        <c:crossAx val="98575853"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -43674,11 +43707,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="71998275"/>
-        <c:axId val="84099624"/>
+        <c:axId val="95406561"/>
+        <c:axId val="67673513"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71998275"/>
+        <c:axId val="95406561"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -43713,14 +43746,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84099624"/>
+        <c:crossAx val="67673513"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84099624"/>
+        <c:axId val="67673513"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -43735,7 +43768,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -43764,7 +43797,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71998275"/>
+        <c:crossAx val="95406561"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -45771,11 +45804,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="62307269"/>
-        <c:axId val="64028799"/>
+        <c:axId val="99586628"/>
+        <c:axId val="95723661"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="62307269"/>
+        <c:axId val="99586628"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -45810,14 +45843,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64028799"/>
+        <c:crossAx val="95723661"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64028799"/>
+        <c:axId val="95723661"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -45832,7 +45865,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -45861,7 +45894,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62307269"/>
+        <c:crossAx val="99586628"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -53994,11 +54027,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="37769256"/>
-        <c:axId val="13828958"/>
+        <c:axId val="72921281"/>
+        <c:axId val="63520717"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="37769256"/>
+        <c:axId val="72921281"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -54033,14 +54066,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13828958"/>
+        <c:crossAx val="63520717"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13828958"/>
+        <c:axId val="63520717"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -54055,7 +54088,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -54084,7 +54117,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37769256"/>
+        <c:crossAx val="72921281"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -56141,11 +56174,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="40273517"/>
-        <c:axId val="97218976"/>
+        <c:axId val="73665686"/>
+        <c:axId val="47957664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40273517"/>
+        <c:axId val="73665686"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -56180,14 +56213,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="97218976"/>
+        <c:crossAx val="47957664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97218976"/>
+        <c:axId val="47957664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -56202,7 +56235,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -56231,7 +56264,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40273517"/>
+        <c:crossAx val="73665686"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -56314,9 +56347,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -56329,7 +56360,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56340,7 +56371,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56349,9 +56380,7 @@
             <c:idx val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -56364,7 +56393,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56373,11 +56402,9 @@
             <c:idx val="5"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56399,7 +56426,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56408,9 +56435,7 @@
             <c:idx val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -56423,7 +56448,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56432,11 +56457,9 @@
             <c:idx val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56445,9 +56468,7 @@
             <c:idx val="11"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -56458,9 +56479,7 @@
             <c:idx val="12"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -56473,7 +56492,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56484,7 +56503,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56493,9 +56512,7 @@
             <c:idx val="15"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -56508,7 +56525,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56517,11 +56534,9 @@
             <c:idx val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56543,7 +56558,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56552,9 +56567,7 @@
             <c:idx val="20"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -56567,7 +56580,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56576,11 +56589,9 @@
             <c:idx val="22"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56589,9 +56600,7 @@
             <c:idx val="23"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -56602,9 +56611,7 @@
             <c:idx val="24"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -56617,7 +56624,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56628,7 +56635,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56637,9 +56644,7 @@
             <c:idx val="27"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -56652,7 +56657,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56661,11 +56666,9 @@
             <c:idx val="29"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56687,7 +56690,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56696,9 +56699,7 @@
             <c:idx val="32"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -56711,7 +56712,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56720,11 +56721,9 @@
             <c:idx val="34"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56733,9 +56732,7 @@
             <c:idx val="35"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -56746,9 +56743,7 @@
             <c:idx val="36"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -56761,7 +56756,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56772,7 +56767,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56781,9 +56776,7 @@
             <c:idx val="39"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -56796,7 +56789,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56805,11 +56798,9 @@
             <c:idx val="41"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56831,7 +56822,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56840,9 +56831,7 @@
             <c:idx val="44"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -56855,7 +56844,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56864,11 +56853,9 @@
             <c:idx val="46"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56877,9 +56864,7 @@
             <c:idx val="47"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -56890,9 +56875,7 @@
             <c:idx val="48"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -56905,7 +56888,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56916,7 +56899,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56925,9 +56908,7 @@
             <c:idx val="51"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -56940,7 +56921,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56949,11 +56930,9 @@
             <c:idx val="53"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56975,7 +56954,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -56984,9 +56963,7 @@
             <c:idx val="56"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -56999,7 +56976,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57008,11 +56985,9 @@
             <c:idx val="58"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57021,9 +56996,7 @@
             <c:idx val="59"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -57034,9 +57007,7 @@
             <c:idx val="60"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -57049,7 +57020,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57060,7 +57031,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57069,9 +57040,7 @@
             <c:idx val="63"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -57084,7 +57053,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57093,11 +57062,9 @@
             <c:idx val="65"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57119,7 +57086,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57128,9 +57095,7 @@
             <c:idx val="68"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -57143,7 +57108,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57152,11 +57117,9 @@
             <c:idx val="70"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57165,9 +57128,7 @@
             <c:idx val="71"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -57178,9 +57139,7 @@
             <c:idx val="72"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -57193,7 +57152,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57204,7 +57163,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57213,9 +57172,7 @@
             <c:idx val="75"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -57228,7 +57185,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57237,11 +57194,9 @@
             <c:idx val="77"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57263,7 +57218,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57272,9 +57227,7 @@
             <c:idx val="80"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -57287,7 +57240,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57296,11 +57249,9 @@
             <c:idx val="82"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57309,9 +57260,7 @@
             <c:idx val="83"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -57322,9 +57271,7 @@
             <c:idx val="84"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -57337,7 +57284,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57348,7 +57295,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57357,9 +57304,7 @@
             <c:idx val="87"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -57372,7 +57317,7 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57381,11 +57326,9 @@
             <c:idx val="89"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="83caff">
-                  <a:alpha val="-47148408"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="3109385880">
+                <a:srgbClr val="83caff"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57407,7 +57350,7 @@
               <a:solidFill>
                 <a:srgbClr val="aecf00"/>
               </a:solidFill>
-              <a:ln w="4124252160">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57416,9 +57359,7 @@
             <c:idx val="92"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4b1f6f">
-                  <a:alpha val="-628179704"/>
-                </a:srgbClr>
+                <a:srgbClr val="4b1f6f"/>
               </a:solidFill>
               <a:ln w="1772368920">
                 <a:noFill/>
@@ -57431,7 +57372,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff950e"/>
               </a:solidFill>
-              <a:ln w="6029941680">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57440,11 +57381,9 @@
             <c:idx val="94"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="c5000b">
-                  <a:alpha val="-25601112"/>
-                </a:srgbClr>
-              </a:solidFill>
-              <a:ln w="4647817080">
+                <a:srgbClr val="c5000b"/>
+              </a:solidFill>
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57453,9 +57392,7 @@
             <c:idx val="95"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0084d1">
-                  <a:alpha val="-33901000"/>
-                </a:srgbClr>
+                <a:srgbClr val="0084d1"/>
               </a:solidFill>
               <a:ln w="12240360">
                 <a:noFill/>
@@ -57466,9 +57403,7 @@
             <c:idx val="96"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="004586">
-                  <a:alpha val="-17698000"/>
-                </a:srgbClr>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:ln w="6407280">
                 <a:noFill/>
@@ -57481,7 +57416,7 @@
               <a:solidFill>
                 <a:srgbClr val="ff420e"/>
               </a:solidFill>
-              <a:ln w="6022292400">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57492,7 +57427,7 @@
               <a:solidFill>
                 <a:srgbClr val="ffd320"/>
               </a:solidFill>
-              <a:ln w="6035662080">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
@@ -57501,9 +57436,7 @@
             <c:idx val="99"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="579d1c">
-                  <a:alpha val="-1446784704"/>
-                </a:srgbClr>
+                <a:srgbClr val="579d1c"/>
               </a:solidFill>
               <a:ln w="2067066720">
                 <a:noFill/>
@@ -57516,12 +57449,921 @@
               <a:solidFill>
                 <a:srgbClr val="7e0021"/>
               </a:solidFill>
-              <a:ln w="2972724840">
+              <a:ln>
                 <a:noFill/>
               </a:ln>
             </c:spPr>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="12"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="13"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="14"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="15"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="16"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="17"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="18"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="19"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="20"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="21"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="22"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="23"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="24"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="25"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="26"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="27"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="28"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="29"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="30"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="31"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="32"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="33"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="34"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="35"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="36"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="37"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="38"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="39"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="40"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="41"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="42"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="43"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="44"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="45"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="46"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="47"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="48"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="49"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="50"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="51"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="52"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="53"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="54"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="55"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="56"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="57"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="58"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="59"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="60"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="61"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="62"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="63"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="64"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="65"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="66"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="67"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="68"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="69"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="70"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="71"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="72"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="73"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="74"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="75"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="76"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="77"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="78"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="79"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="80"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="81"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="82"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="83"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="84"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="85"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="86"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="87"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="88"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="89"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="90"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="91"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="92"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="93"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="94"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="95"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="96"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="97"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="98"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="99"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="100"/>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+            </c:dLbl>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
@@ -58163,11 +59005,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="47820889"/>
-        <c:axId val="89255824"/>
+        <c:axId val="24976029"/>
+        <c:axId val="67423320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47820889"/>
+        <c:axId val="24976029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -58202,14 +59044,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89255824"/>
+        <c:crossAx val="67423320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89255824"/>
+        <c:axId val="67423320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -58235,7 +59077,7 @@
             </a:ln>
           </c:spPr>
         </c:minorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -58264,7 +59106,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47820889"/>
+        <c:crossAx val="24976029"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -60271,11 +61113,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="94152856"/>
-        <c:axId val="40688623"/>
+        <c:axId val="30313682"/>
+        <c:axId val="15618268"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="94152856"/>
+        <c:axId val="30313682"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -60310,14 +61152,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40688623"/>
+        <c:crossAx val="15618268"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40688623"/>
+        <c:axId val="15618268"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -60332,7 +61174,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -60361,7 +61203,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94152856"/>
+        <c:crossAx val="30313682"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -68494,11 +69336,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="27675182"/>
-        <c:axId val="14636465"/>
+        <c:axId val="914895"/>
+        <c:axId val="68037871"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27675182"/>
+        <c:axId val="914895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -68533,14 +69375,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14636465"/>
+        <c:crossAx val="68037871"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14636465"/>
+        <c:axId val="68037871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -68555,7 +69397,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -68584,7 +69426,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27675182"/>
+        <c:crossAx val="914895"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -68632,9 +69474,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>208080</xdr:colOff>
+      <xdr:colOff>206640</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>96120</xdr:rowOff>
+      <xdr:rowOff>94680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68643,7 +69485,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="277560" y="3274560"/>
-        <a:ext cx="7864560" cy="5599800"/>
+        <a:ext cx="7301160" cy="5598360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68662,9 +69504,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>323280</xdr:colOff>
+      <xdr:colOff>321840</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>49680</xdr:rowOff>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68672,8 +69514,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8235360" y="3274560"/>
-        <a:ext cx="10623240" cy="5390640"/>
+        <a:off x="7673400" y="3274560"/>
+        <a:ext cx="9926640" cy="5389200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68692,9 +69534,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>399240</xdr:colOff>
+      <xdr:colOff>397800</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68702,8 +69544,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="370800" y="8633160"/>
-        <a:ext cx="16449480" cy="4470120"/>
+        <a:off x="332640" y="8633160"/>
+        <a:ext cx="15381360" cy="4468680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68727,9 +69569,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>11880</xdr:colOff>
+      <xdr:colOff>10440</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68738,7 +69580,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="81000" y="1076400"/>
-        <a:ext cx="8017560" cy="5599800"/>
+        <a:ext cx="7454160" cy="5598360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68757,9 +69599,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>33120</xdr:colOff>
+      <xdr:colOff>31680</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68767,8 +69609,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8097480" y="1029960"/>
-        <a:ext cx="10623600" cy="5317920"/>
+        <a:off x="7535520" y="1029960"/>
+        <a:ext cx="9926640" cy="5316480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68787,9 +69629,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>133560</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+      <xdr:rowOff>153720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68798,7 +69640,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="388080" y="6490800"/>
-        <a:ext cx="16814160" cy="4393080"/>
+        <a:ext cx="15669720" cy="4391640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68817,14 +69659,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>175680</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>111240</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:colOff>109800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>58680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68832,8 +69674,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="175680" y="619560"/>
-        <a:ext cx="17556480" cy="4363200"/>
+        <a:off x="175680" y="743760"/>
+        <a:ext cx="16374240" cy="4361760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68850,16 +69692,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>441000</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2880</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>74880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>372240</xdr:colOff>
+      <xdr:colOff>370800</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68868,7 +69710,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="441000" y="1050120"/>
-        <a:ext cx="8017920" cy="4949280"/>
+        <a:ext cx="7454520" cy="4947840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68887,9 +69729,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>321120</xdr:colOff>
+      <xdr:colOff>319680</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>6840</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68897,8 +69739,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8385840" y="1028880"/>
-        <a:ext cx="10623240" cy="4992480"/>
+        <a:off x="7823880" y="1028880"/>
+        <a:ext cx="9926280" cy="4991040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68917,9 +69759,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>133560</xdr:colOff>
+      <xdr:colOff>132120</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -68928,7 +69770,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="388080" y="6201720"/>
-        <a:ext cx="16814160" cy="4068000"/>
+        <a:ext cx="15669720" cy="4066560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -68954,47 +69796,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69212,47 +70051,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69298,55 +70134,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C2"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -69357,12 +70190,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
+    <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="n">
+      <c r="C2" s="7" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <f aca="false">MAX(C2:MM2)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="str">
+        <f aca="false">HLOOKUP(C4,C2:MM3,2,1)</f>
+        <v>Random</v>
       </c>
     </row>
   </sheetData>
@@ -69390,52 +70245,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="6.20918367346939"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="31" min="30" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="7.4234693877551"/>
     <col collapsed="false" hidden="false" max="37" min="37" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.3469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="44" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -69452,14 +70304,14 @@
         <v>4</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="11"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>